<commit_message>
Remove old tracing files
</commit_message>
<xml_diff>
--- a/analized-output/StreamLine Data.xlsx
+++ b/analized-output/StreamLine Data.xlsx
@@ -554,11 +554,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="627883464"/>
-        <c:axId val="627892872"/>
+        <c:axId val="604487520"/>
+        <c:axId val="604483992"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="627883464"/>
+        <c:axId val="604487520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -601,7 +601,7 @@
             <a:endParaRPr lang="ko-KR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="627892872"/>
+        <c:crossAx val="604483992"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -609,7 +609,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="627892872"/>
+        <c:axId val="604483992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -660,7 +660,7 @@
             <a:endParaRPr lang="ko-KR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="627883464"/>
+        <c:crossAx val="604487520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1065,11 +1065,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="627898360"/>
-        <c:axId val="627899144"/>
+        <c:axId val="604485168"/>
+        <c:axId val="604487912"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="627898360"/>
+        <c:axId val="604485168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1112,7 +1112,7 @@
             <a:endParaRPr lang="ko-KR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="627899144"/>
+        <c:crossAx val="604487912"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1120,7 +1120,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="627899144"/>
+        <c:axId val="604487912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1171,7 +1171,7 @@
             <a:endParaRPr lang="ko-KR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="627898360"/>
+        <c:crossAx val="604485168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1502,11 +1502,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="627897184"/>
-        <c:axId val="627889344"/>
+        <c:axId val="604483208"/>
+        <c:axId val="604486736"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="627897184"/>
+        <c:axId val="604483208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1549,7 +1549,7 @@
             <a:endParaRPr lang="ko-KR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="627889344"/>
+        <c:crossAx val="604486736"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1557,7 +1557,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="627889344"/>
+        <c:axId val="604486736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1608,7 +1608,7 @@
             <a:endParaRPr lang="ko-KR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="627897184"/>
+        <c:crossAx val="604483208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1935,11 +1935,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="627898752"/>
-        <c:axId val="627897576"/>
+        <c:axId val="604488304"/>
+        <c:axId val="604487128"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="627898752"/>
+        <c:axId val="604488304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1982,7 +1982,7 @@
             <a:endParaRPr lang="ko-KR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="627897576"/>
+        <c:crossAx val="604487128"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1990,7 +1990,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="627897576"/>
+        <c:axId val="604487128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2041,7 +2041,7 @@
             <a:endParaRPr lang="ko-KR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="627898752"/>
+        <c:crossAx val="604488304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2353,11 +2353,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="627893264"/>
-        <c:axId val="627899536"/>
+        <c:axId val="604488696"/>
+        <c:axId val="604490656"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="627893264"/>
+        <c:axId val="604488696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2414,7 +2414,7 @@
             <a:endParaRPr lang="ko-KR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="627899536"/>
+        <c:crossAx val="604490656"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2422,7 +2422,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="627899536"/>
+        <c:axId val="604490656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2479,7 +2479,7 @@
             <a:endParaRPr lang="ko-KR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="627893264"/>
+        <c:crossAx val="604488696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2791,11 +2791,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="627900320"/>
-        <c:axId val="627888560"/>
+        <c:axId val="604481640"/>
+        <c:axId val="604482032"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="627900320"/>
+        <c:axId val="604481640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2852,7 +2852,7 @@
             <a:endParaRPr lang="ko-KR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="627888560"/>
+        <c:crossAx val="604482032"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2860,7 +2860,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="627888560"/>
+        <c:axId val="604482032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2917,7 +2917,7 @@
             <a:endParaRPr lang="ko-KR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="627900320"/>
+        <c:crossAx val="604481640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3238,11 +3238,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="627888168"/>
-        <c:axId val="627894048"/>
+        <c:axId val="604482816"/>
+        <c:axId val="604495360"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="627888168"/>
+        <c:axId val="604482816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3299,7 +3299,7 @@
             <a:endParaRPr lang="ko-KR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="627894048"/>
+        <c:crossAx val="604495360"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3307,7 +3307,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="627894048"/>
+        <c:axId val="604495360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3364,7 +3364,7 @@
             <a:endParaRPr lang="ko-KR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="627888168"/>
+        <c:crossAx val="604482816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7313,7 +7313,7 @@
         <xdr:cNvPr id="3" name="차트 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{FA55E663-4874-433B-94E5-C96DA2DA277B}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FA55E663-4874-433B-94E5-C96DA2DA277B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7349,7 +7349,7 @@
         <xdr:cNvPr id="6" name="차트 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{F48BE1A5-969F-4248-91D5-CD4CE75327D0}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F48BE1A5-969F-4248-91D5-CD4CE75327D0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7385,7 +7385,7 @@
         <xdr:cNvPr id="7" name="차트 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{1C280A80-7593-4CE3-AEEB-6B2C1E4A0EAB}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1C280A80-7593-4CE3-AEEB-6B2C1E4A0EAB}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7423,7 +7423,7 @@
         <xdr:cNvPr id="8" name="차트 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{3F279ADD-33AB-42E8-AA48-FDF303586B51}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3F279ADD-33AB-42E8-AA48-FDF303586B51}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7461,7 +7461,7 @@
         <xdr:cNvPr id="12" name="차트 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{2BDBF86D-8E2A-421F-8128-87793D7E1B53}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2BDBF86D-8E2A-421F-8128-87793D7E1B53}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7497,7 +7497,7 @@
         <xdr:cNvPr id="13" name="차트 12">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{CC8EC645-36E5-4DC7-8E2F-C78F5F84EE56}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CC8EC645-36E5-4DC7-8E2F-C78F5F84EE56}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7535,7 +7535,7 @@
         <xdr:cNvPr id="14" name="차트 13">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E7305D1A-8FDC-4A38-8068-8C599C6C4258}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E7305D1A-8FDC-4A38-8068-8C599C6C4258}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7857,8 +7857,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AG21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="L50" sqref="L50"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AD47" sqref="AD47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>

</xml_diff>